<commit_message>
add profit taker in backtesting
</commit_message>
<xml_diff>
--- a/portfolios/sml_equity/profit_reports/trend/Bollinger_overall.xlsx
+++ b/portfolios/sml_equity/profit_reports/trend/Bollinger_overall.xlsx
@@ -465,46 +465,46 @@
     </row>
     <row r="2" spans="1:14">
       <c r="A2">
-        <v>5624</v>
+        <v>4845</v>
       </c>
       <c r="B2">
-        <v>7953</v>
+        <v>7408</v>
       </c>
       <c r="C2">
-        <v>13577</v>
+        <v>12253</v>
       </c>
       <c r="D2">
-        <v>1946.485605626239</v>
+        <v>2160.618445841338</v>
       </c>
       <c r="E2">
-        <v>-969.5492190974893</v>
+        <v>-964.7371519586635</v>
       </c>
       <c r="F2">
-        <v>0.1954806507590645</v>
+        <v>0.2171133938593462</v>
       </c>
       <c r="G2">
-        <v>-0.09602502398511337</v>
+        <v>-0.09550606636550885</v>
       </c>
       <c r="H2">
-        <v>0.02472535642007594</v>
+        <v>0.02810784735271694</v>
       </c>
       <c r="I2">
-        <v>10947035.046042</v>
+        <v>10468196.37010127</v>
       </c>
       <c r="J2">
-        <v>-7710824.939482331</v>
+        <v>-7146772.821709784</v>
       </c>
       <c r="K2">
-        <v>0.4142299477056787</v>
+        <v>0.3954133681547376</v>
       </c>
       <c r="L2">
-        <v>2.007619177330818</v>
+        <v>2.239592868850058</v>
       </c>
       <c r="M2">
-        <v>1.419697001547662</v>
+        <v>1.464744526131009</v>
       </c>
       <c r="N2">
-        <v>3236210.106559664</v>
+        <v>3321423.548391489</v>
       </c>
     </row>
   </sheetData>

</xml_diff>